<commit_message>
check in updates to TrusteeEP05 and Poll Coverage
check in updates to TrusteeEP05 and Poll Coverage
</commit_message>
<xml_diff>
--- a/campaign/TrusteeEP_05/Poll Coverage Tooba.xlsx
+++ b/campaign/TrusteeEP_05/Poll Coverage Tooba.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21520" windowHeight="15340" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -28,8 +28,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -68,6 +68,79 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -79,7 +152,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="78DC78"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -390,21 +463,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -413,7 +486,7 @@
         <v>0.29255319148936171</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -422,7 +495,7 @@
         <v>3.140096618357488E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -431,7 +504,7 @@
         <v>2.7397260273972601E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -439,7 +512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -447,7 +520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -456,7 +529,7 @@
         <v>6.9408740359897178E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -464,7 +537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -472,7 +545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -480,7 +553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -488,7 +561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -497,7 +570,7 @@
         <v>6.1488673139158574E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -506,7 +579,7 @@
         <v>0.32577903682719545</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -515,7 +588,7 @@
         <v>0.57076566125290018</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -524,7 +597,7 @@
         <v>2.4305555555555556E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -533,7 +606,7 @@
         <v>7.3863636363636367E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -542,7 +615,7 @@
         <v>9.3023255813953487E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -550,7 +623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -558,7 +631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -567,7 +640,7 @@
         <v>4.0123456790123455E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -576,7 +649,7 @@
         <v>0.20527859237536658</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -585,7 +658,7 @@
         <v>4.434589800443459E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <f>A23+1</f>
         <v>22</v>
@@ -595,9 +668,9 @@
         <v>0.16120218579234974</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
-        <f t="shared" ref="A25:A49" si="0">A24+1</f>
+        <f t="shared" ref="A25:A43" si="0">A24+1</f>
         <v>23</v>
       </c>
       <c r="B25" s="1">
@@ -605,7 +678,7 @@
         <v>0.44504021447721182</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -615,7 +688,7 @@
         <v>0.17732558139534885</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -625,7 +698,7 @@
         <v>8.8397790055248615E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -635,7 +708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -645,7 +718,7 @@
         <v>3.6956521739130437E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -655,7 +728,7 @@
         <v>0.13943355119825709</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -664,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -673,7 +746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -682,7 +755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -692,7 +765,7 @@
         <v>1.8604651162790697E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -702,7 +775,7 @@
         <v>1.3262599469496022E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -712,7 +785,7 @@
         <v>1.1881188118811881E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -721,7 +794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -731,7 +804,7 @@
         <v>3.0441400304414001E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -741,16 +814,16 @@
         <v>0.12133072407045009</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="B40" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -759,7 +832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -769,7 +842,7 @@
         <v>0.61443932411674351</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -780,10 +853,9 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>

</xml_diff>